<commit_message>
Updated MemoryLab for new server
</commit_message>
<xml_diff>
--- a/MemoryLab/starter-code/CacheCharts.xlsx
+++ b/MemoryLab/starter-code/CacheCharts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/personal-version-control/phsi_supplements/labs/10.memorylab/starter-code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/textbook/labs/MemoryLab/starter-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77869D98-DAA4-A943-AB3A-5EBB5A5D0F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CD752F-AC2C-AD49-A3DD-0B9147EAF9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46980" yWindow="-440" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{C93E0F98-7BD9-504A-8311-46AFA0E4279F}"/>
+    <workbookView xWindow="920" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{C93E0F98-7BD9-504A-8311-46AFA0E4279F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cache Size" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Data Extraction" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Data!$G$2:$G$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Data!$G$2:$G$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="83">
   <si>
     <t>CACHE SIZE</t>
   </si>
@@ -256,6 +256,39 @@
   </si>
   <si>
     <t>Time spent working with data when stride is 2 bytes: 0.90 sec.</t>
+  </si>
+  <si>
+    <t>40 MB</t>
+  </si>
+  <si>
+    <t>48 MB</t>
+  </si>
+  <si>
+    <t>64 MB</t>
+  </si>
+  <si>
+    <t>80 MB</t>
+  </si>
+  <si>
+    <t>96 MB</t>
+  </si>
+  <si>
+    <t>128 MB</t>
+  </si>
+  <si>
+    <t>160 MB</t>
+  </si>
+  <si>
+    <t>192 MB</t>
+  </si>
+  <si>
+    <t>256 MB</t>
+  </si>
+  <si>
+    <t>320 MB</t>
+  </si>
+  <si>
+    <t>384 MB</t>
   </si>
 </sst>
 </file>
@@ -368,9 +401,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$56</c:f>
+              <c:f>Data!$A$2:$A$67</c:f>
               <c:strCache>
-                <c:ptCount val="55"/>
+                <c:ptCount val="66"/>
                 <c:pt idx="0">
                   <c:v>128 bytes</c:v>
                 </c:pt>
@@ -535,16 +568,49 @@
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>40 MB</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>48 MB</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>80 MB</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>96 MB</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>128 MB</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>160 MB</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>192 MB</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>256 MB</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>320 MB</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>384 MB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$56</c:f>
+              <c:f>Data!$B$2:$B$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="66"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -708,6 +774,39 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="54">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="65">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -801,8 +900,8 @@
         <c:axId val="1764424976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4"/>
-          <c:min val="1"/>
+          <c:max val="3"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -939,7 +1038,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$64:$A$74</c:f>
+              <c:f>Data!$A$75:$A$85</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -980,7 +1079,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$64:$B$74</c:f>
+              <c:f>Data!$B$75:$B$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1094,6 +1193,7 @@
         <c:axId val="1761707616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2309,7 +2409,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3BD96459-FB1C-7448-AA1A-BA3878C2493A}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="161" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2690,11 +2790,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA063B1-BC06-DD46-BF81-9C28C7BAF327}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2751,7 +2849,7 @@
         <v>43</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B56" si="0">(C3+D3+E3+F3+G3-MAX(C3:G3)-MIN(C3:G3))/3</f>
+        <f t="shared" ref="B3:B67" si="0">(C3+D3+E3+F3+G3-MAX(C3:G3)-MIN(C3:G3))/3</f>
         <v>100</v>
       </c>
       <c r="C3">
@@ -3851,7 +3949,7 @@
         <v>31</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B47:B57" si="1">(C47+D47+E47+F47+G47-MAX(C47:G47)-MIN(C47:G47))/3</f>
         <v>100</v>
       </c>
       <c r="C47">
@@ -3876,7 +3974,7 @@
         <v>58</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C48">
@@ -3901,7 +3999,7 @@
         <v>32</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C49">
@@ -3926,7 +4024,7 @@
         <v>59</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C50">
@@ -3951,7 +4049,7 @@
         <v>60</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C51">
@@ -3976,7 +4074,7 @@
         <v>61</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C52">
@@ -4001,7 +4099,7 @@
         <v>62</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C53">
@@ -4026,7 +4124,7 @@
         <v>68</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C54">
@@ -4051,7 +4149,7 @@
         <v>69</v>
       </c>
       <c r="B55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C55">
@@ -4076,7 +4174,7 @@
         <v>67</v>
       </c>
       <c r="B56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="C56">
@@ -4097,301 +4195,576 @@
       <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G57" s="1"/>
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="C57">
+        <v>100</v>
+      </c>
+      <c r="D57">
+        <v>100</v>
+      </c>
+      <c r="E57">
+        <v>100</v>
+      </c>
+      <c r="F57">
+        <v>100</v>
+      </c>
+      <c r="G57">
+        <v>100</v>
+      </c>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G58" s="1"/>
+      <c r="A58" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C58">
+        <v>100</v>
+      </c>
+      <c r="D58">
+        <v>100</v>
+      </c>
+      <c r="E58">
+        <v>100</v>
+      </c>
+      <c r="F58">
+        <v>100</v>
+      </c>
+      <c r="G58">
+        <v>100</v>
+      </c>
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G59" s="1"/>
+      <c r="A59" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C59">
+        <v>100</v>
+      </c>
+      <c r="D59">
+        <v>100</v>
+      </c>
+      <c r="E59">
+        <v>100</v>
+      </c>
+      <c r="F59">
+        <v>100</v>
+      </c>
+      <c r="G59">
+        <v>100</v>
+      </c>
       <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C60">
+        <v>100</v>
+      </c>
+      <c r="D60">
+        <v>100</v>
+      </c>
+      <c r="E60">
+        <v>100</v>
+      </c>
+      <c r="F60">
+        <v>100</v>
+      </c>
+      <c r="G60">
+        <v>100</v>
+      </c>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C61">
+        <v>100</v>
+      </c>
+      <c r="D61">
+        <v>100</v>
+      </c>
+      <c r="E61">
+        <v>100</v>
+      </c>
+      <c r="F61">
+        <v>100</v>
+      </c>
+      <c r="G61">
+        <v>100</v>
+      </c>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C62">
+        <v>100</v>
+      </c>
+      <c r="D62">
+        <v>100</v>
+      </c>
+      <c r="E62">
+        <v>100</v>
+      </c>
+      <c r="F62">
+        <v>100</v>
+      </c>
+      <c r="G62">
+        <v>100</v>
+      </c>
+      <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>34</v>
-      </c>
-      <c r="B63" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C63">
+        <v>100</v>
+      </c>
+      <c r="D63">
+        <v>100</v>
+      </c>
+      <c r="E63">
+        <v>100</v>
+      </c>
+      <c r="F63">
+        <v>100</v>
+      </c>
+      <c r="G63">
+        <v>100</v>
+      </c>
+      <c r="I63" s="1"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C64">
+        <v>100</v>
+      </c>
+      <c r="D64">
+        <v>100</v>
+      </c>
+      <c r="E64">
+        <v>100</v>
+      </c>
+      <c r="F64">
+        <v>100</v>
+      </c>
+      <c r="G64">
+        <v>100</v>
+      </c>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C65">
+        <v>100</v>
+      </c>
+      <c r="D65">
+        <v>100</v>
+      </c>
+      <c r="E65">
+        <v>100</v>
+      </c>
+      <c r="F65">
+        <v>100</v>
+      </c>
+      <c r="G65">
+        <v>100</v>
+      </c>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C66">
+        <v>100</v>
+      </c>
+      <c r="D66">
+        <v>100</v>
+      </c>
+      <c r="E66">
+        <v>100</v>
+      </c>
+      <c r="F66">
+        <v>100</v>
+      </c>
+      <c r="G66">
+        <v>100</v>
+      </c>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>82</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C67">
+        <v>100</v>
+      </c>
+      <c r="D67">
+        <v>100</v>
+      </c>
+      <c r="E67">
+        <v>100</v>
+      </c>
+      <c r="F67">
+        <v>100</v>
+      </c>
+      <c r="G67">
+        <v>100</v>
+      </c>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G69" s="1"/>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>35</v>
       </c>
-      <c r="B64">
-        <f t="shared" ref="B64:B74" si="1">(C64+D64+E64+F64+G64-MAX(C64:G64)-MIN(C64:G64))/3</f>
-        <v>100</v>
-      </c>
-      <c r="C64">
-        <v>100</v>
-      </c>
-      <c r="D64">
-        <v>100</v>
-      </c>
-      <c r="E64">
-        <v>100</v>
-      </c>
-      <c r="F64">
-        <v>100</v>
-      </c>
-      <c r="G64">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="B75">
+        <f t="shared" ref="B75:B85" si="2">(C75+D75+E75+F75+G75-MAX(C75:G75)-MIN(C75:G75))/3</f>
+        <v>100</v>
+      </c>
+      <c r="C75">
+        <v>100</v>
+      </c>
+      <c r="D75">
+        <v>100</v>
+      </c>
+      <c r="E75">
+        <v>100</v>
+      </c>
+      <c r="F75">
+        <v>100</v>
+      </c>
+      <c r="G75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>36</v>
       </c>
-      <c r="B65">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C65">
-        <v>100</v>
-      </c>
-      <c r="D65">
-        <v>100</v>
-      </c>
-      <c r="E65">
-        <v>100</v>
-      </c>
-      <c r="F65">
-        <v>100</v>
-      </c>
-      <c r="G65">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="B76">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C76">
+        <v>100</v>
+      </c>
+      <c r="D76">
+        <v>100</v>
+      </c>
+      <c r="E76">
+        <v>100</v>
+      </c>
+      <c r="F76">
+        <v>100</v>
+      </c>
+      <c r="G76">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>37</v>
       </c>
-      <c r="B66">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C66">
-        <v>100</v>
-      </c>
-      <c r="D66">
-        <v>100</v>
-      </c>
-      <c r="E66">
-        <v>100</v>
-      </c>
-      <c r="F66">
-        <v>100</v>
-      </c>
-      <c r="G66">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B77">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C77">
+        <v>100</v>
+      </c>
+      <c r="D77">
+        <v>100</v>
+      </c>
+      <c r="E77">
+        <v>100</v>
+      </c>
+      <c r="F77">
+        <v>100</v>
+      </c>
+      <c r="G77">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>38</v>
       </c>
-      <c r="B67">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C67">
-        <v>100</v>
-      </c>
-      <c r="D67">
-        <v>100</v>
-      </c>
-      <c r="E67">
-        <v>100</v>
-      </c>
-      <c r="F67">
-        <v>100</v>
-      </c>
-      <c r="G67">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="B78">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C78">
+        <v>100</v>
+      </c>
+      <c r="D78">
+        <v>100</v>
+      </c>
+      <c r="E78">
+        <v>100</v>
+      </c>
+      <c r="F78">
+        <v>100</v>
+      </c>
+      <c r="G78">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>39</v>
       </c>
-      <c r="B68">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C68">
-        <v>100</v>
-      </c>
-      <c r="D68">
-        <v>100</v>
-      </c>
-      <c r="E68">
-        <v>100</v>
-      </c>
-      <c r="F68">
-        <v>100</v>
-      </c>
-      <c r="G68">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B79">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C79">
+        <v>100</v>
+      </c>
+      <c r="D79">
+        <v>100</v>
+      </c>
+      <c r="E79">
+        <v>100</v>
+      </c>
+      <c r="F79">
+        <v>100</v>
+      </c>
+      <c r="G79">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>40</v>
       </c>
-      <c r="B69">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C69">
-        <v>100</v>
-      </c>
-      <c r="D69">
-        <v>100</v>
-      </c>
-      <c r="E69">
-        <v>100</v>
-      </c>
-      <c r="F69">
-        <v>100</v>
-      </c>
-      <c r="G69">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="B80">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C80">
+        <v>100</v>
+      </c>
+      <c r="D80">
+        <v>100</v>
+      </c>
+      <c r="E80">
+        <v>100</v>
+      </c>
+      <c r="F80">
+        <v>100</v>
+      </c>
+      <c r="G80">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>1</v>
       </c>
-      <c r="B70">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C70">
-        <v>100</v>
-      </c>
-      <c r="D70">
-        <v>100</v>
-      </c>
-      <c r="E70">
-        <v>100</v>
-      </c>
-      <c r="F70">
-        <v>100</v>
-      </c>
-      <c r="G70">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B81">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C81">
+        <v>100</v>
+      </c>
+      <c r="D81">
+        <v>100</v>
+      </c>
+      <c r="E81">
+        <v>100</v>
+      </c>
+      <c r="F81">
+        <v>100</v>
+      </c>
+      <c r="G81">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>3</v>
       </c>
-      <c r="B71">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C71">
-        <v>100</v>
-      </c>
-      <c r="D71">
-        <v>100</v>
-      </c>
-      <c r="E71">
-        <v>100</v>
-      </c>
-      <c r="F71">
-        <v>100</v>
-      </c>
-      <c r="G71">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="B82">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C82">
+        <v>100</v>
+      </c>
+      <c r="D82">
+        <v>100</v>
+      </c>
+      <c r="E82">
+        <v>100</v>
+      </c>
+      <c r="F82">
+        <v>100</v>
+      </c>
+      <c r="G82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>5</v>
       </c>
-      <c r="B72">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C72">
-        <v>100</v>
-      </c>
-      <c r="D72">
-        <v>100</v>
-      </c>
-      <c r="E72">
-        <v>100</v>
-      </c>
-      <c r="F72">
-        <v>100</v>
-      </c>
-      <c r="G72">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="B83">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C83">
+        <v>100</v>
+      </c>
+      <c r="D83">
+        <v>100</v>
+      </c>
+      <c r="E83">
+        <v>100</v>
+      </c>
+      <c r="F83">
+        <v>100</v>
+      </c>
+      <c r="G83">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>41</v>
       </c>
-      <c r="B73">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C73">
-        <v>100</v>
-      </c>
-      <c r="D73">
-        <v>100</v>
-      </c>
-      <c r="E73">
-        <v>100</v>
-      </c>
-      <c r="F73">
-        <v>100</v>
-      </c>
-      <c r="G73">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="B84">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C84">
+        <v>100</v>
+      </c>
+      <c r="D84">
+        <v>100</v>
+      </c>
+      <c r="E84">
+        <v>100</v>
+      </c>
+      <c r="F84">
+        <v>100</v>
+      </c>
+      <c r="G84">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>42</v>
       </c>
-      <c r="B74">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="C74">
-        <v>100</v>
-      </c>
-      <c r="D74">
-        <v>100</v>
-      </c>
-      <c r="E74">
-        <v>100</v>
-      </c>
-      <c r="F74">
-        <v>100</v>
-      </c>
-      <c r="G74">
+      <c r="B85">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C85">
+        <v>100</v>
+      </c>
+      <c r="D85">
+        <v>100</v>
+      </c>
+      <c r="E85">
+        <v>100</v>
+      </c>
+      <c r="F85">
+        <v>100</v>
+      </c>
+      <c r="G85">
         <v>100</v>
       </c>
     </row>
@@ -4404,7 +4777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB66E5A9-00E7-224D-B37E-C4BDE8B14A62}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>